<commit_message>
Changed cube recipe for Shimmering gc/sc. Added EMF to data.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Diablo II LOD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A18D2EA-57AA-49A6-9ADF-83D3E51AD26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977F8A81-C37D-4B02-AABF-6F93E6658372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="7" xr2:uid="{B5C7FBEC-5C21-4BB4-BF82-AC400E45706D}"/>
+    <workbookView xWindow="-28920" yWindow="7620" windowWidth="29040" windowHeight="15525" activeTab="2" xr2:uid="{B5C7FBEC-5C21-4BB4-BF82-AC400E45706D}"/>
   </bookViews>
   <sheets>
     <sheet name="DropMult" sheetId="1" r:id="rId1"/>
     <sheet name="Set Items" sheetId="3" r:id="rId2"/>
     <sheet name="Unique Items" sheetId="2" r:id="rId3"/>
-    <sheet name="Unique Rings" sheetId="4" r:id="rId4"/>
-    <sheet name="Unique Amulets" sheetId="5" r:id="rId5"/>
-    <sheet name="Rainbow Facets" sheetId="6" r:id="rId6"/>
-    <sheet name="Unique Charms" sheetId="7" r:id="rId7"/>
-    <sheet name="Poison Damage" sheetId="8" r:id="rId8"/>
+    <sheet name="EMF" sheetId="9" r:id="rId4"/>
+    <sheet name="Unique Rings" sheetId="4" r:id="rId5"/>
+    <sheet name="Unique Amulets" sheetId="5" r:id="rId6"/>
+    <sheet name="Rainbow Facets" sheetId="6" r:id="rId7"/>
+    <sheet name="Unique Charms" sheetId="7" r:id="rId8"/>
+    <sheet name="Poison Damage" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="448">
   <si>
     <t>A</t>
   </si>
@@ -1393,6 +1394,22 @@
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>MF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -48251,11 +48268,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D967D6-5472-4C90-A86C-39FA06C9944B}">
   <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U47" sqref="U47"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -49704,6 +49721,2587 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FBE193-D741-4D5C-A5C8-A270E8EA5659}">
+  <dimension ref="A1:D151"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f>INT(IF($A2&lt;10,$A2,$A2*250/($A2+250)))</f>
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <f>INT(IF($A2&lt;10,$A2,$A2*250/($A2+500)))</f>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f>INT(IF($A2&lt;10,$A2,$A2*250/($A2+600)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">INT(IF($A3&lt;10,$A3,$A3*250/($A3+250)))</f>
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="1">INT(IF($A3&lt;10,$A3,$A3*250/($A3+500)))</f>
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="2">INT(IF($A3&lt;10,$A3,$A3*250/($A3+600)))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>120</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>130</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>140</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>150</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>160</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>170</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>180</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>190</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>210</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>220</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>230</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>240</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>250</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>260</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>280</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>290</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>300</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>310</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>320</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>330</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>340</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>350</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>360</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>370</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>380</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>390</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>400</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>410</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>420</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>430</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>440</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>450</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>460</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>470</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>480</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>490</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>500</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>510</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>520</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>530</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>540</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>550</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>560</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>570</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>580</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>590</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>600</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>610</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>620</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>630</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>640</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>650</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>660</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B130" si="3">INT(IF($A67&lt;10,$A67,$A67*250/($A67+250)))</f>
+        <v>181</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="4">INT(IF($A67&lt;10,$A67,$A67*250/($A67+500)))</f>
+        <v>142</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="5">INT(IF($A67&lt;10,$A67,$A67*250/($A67+600)))</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>670</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="3"/>
+        <v>182</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>680</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="3"/>
+        <v>182</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>690</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="3"/>
+        <v>183</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>700</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>184</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>710</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>184</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>720</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>185</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="4"/>
+        <v>147</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>730</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="5"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>740</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="4"/>
+        <v>149</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="5"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>750</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="3"/>
+        <v>187</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="5"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>760</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="5"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>770</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="5"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>780</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="3"/>
+        <v>189</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="5"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>790</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="3"/>
+        <v>189</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="5"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>800</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>810</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>191</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>820</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>191</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>830</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>192</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>840</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>192</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>850</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>193</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>157</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>860</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>193</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>870</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>880</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>159</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>890</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>900</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>910</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>920</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>930</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>940</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>950</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>960</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>970</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>980</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>199</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>990</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>199</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1000</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1010</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1020</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1030</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="4"/>
+        <v>168</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1040</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="4"/>
+        <v>168</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1050</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1060</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1070</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1080</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1090</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="5"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1100</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="5"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1110</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="4"/>
+        <v>172</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="5"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1120</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="4"/>
+        <v>172</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="5"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1130</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="4"/>
+        <v>173</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1140</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="4"/>
+        <v>173</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1150</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1160</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1170</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="5"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1180</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="5"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1190</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="5"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1200</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="5"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1210</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="5"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1220</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="5"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1230</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1240</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1250</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1260</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="5"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1270</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="5"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1280</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1290</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1300</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B151" si="6">INT(IF($A131&lt;10,$A131,$A131*250/($A131+250)))</f>
+        <v>209</v>
+      </c>
+      <c r="C131">
+        <f t="shared" ref="C131:C151" si="7">INT(IF($A131&lt;10,$A131,$A131*250/($A131+500)))</f>
+        <v>180</v>
+      </c>
+      <c r="D131">
+        <f t="shared" ref="D131:D151" si="8">INT(IF($A131&lt;10,$A131,$A131*250/($A131+600)))</f>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1310</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="6"/>
+        <v>209</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="8"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1320</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="7"/>
+        <v>181</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="8"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1330</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="7"/>
+        <v>181</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="8"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1340</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="8"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1350</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="8"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1360</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="6"/>
+        <v>211</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="8"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>1370</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="6"/>
+        <v>211</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="7"/>
+        <v>183</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="8"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1380</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="6"/>
+        <v>211</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="7"/>
+        <v>183</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="8"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1390</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="6"/>
+        <v>211</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="7"/>
+        <v>183</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="8"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1400</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="6"/>
+        <v>212</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="7"/>
+        <v>184</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="8"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1410</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="6"/>
+        <v>212</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="7"/>
+        <v>184</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="8"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>1420</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="6"/>
+        <v>212</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="7"/>
+        <v>184</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="8"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>1430</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="6"/>
+        <v>212</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="7"/>
+        <v>185</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>1440</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="6"/>
+        <v>213</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="7"/>
+        <v>185</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1450</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="6"/>
+        <v>213</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="7"/>
+        <v>185</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1460</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="6"/>
+        <v>213</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="7"/>
+        <v>186</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="8"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1470</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="6"/>
+        <v>213</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="7"/>
+        <v>186</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="8"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1480</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="6"/>
+        <v>213</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="7"/>
+        <v>186</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="8"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>1490</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="6"/>
+        <v>214</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="7"/>
+        <v>187</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="8"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1500</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="6"/>
+        <v>214</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="7"/>
+        <v>187</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="8"/>
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829761FD-4499-474D-94D0-520F26228D2F}">
   <dimension ref="A2:B10"/>
   <sheetViews>
@@ -49797,7 +52395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8208AF0C-A684-4202-BBD6-5A4B78BD1E37}">
   <dimension ref="A2:B13"/>
   <sheetViews>
@@ -49915,7 +52513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83CD3AE-EAA0-4B87-82B2-3F19A0F60658}">
   <dimension ref="A2:C9"/>
   <sheetViews>
@@ -50023,7 +52621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC74B19-CCB5-4585-9D9C-563E439663ED}">
   <dimension ref="A2:B4"/>
   <sheetViews>
@@ -50066,11 +52664,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CE4950-635D-4D71-99C9-E75BB094CED2}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Restored item drop rate from ItemRatio.txt Greatly increased unique and set drop from act bosses, super uniques, unique & champion monsters.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497D4737-808D-4FA6-9B27-CB10500AC47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3618D580-DCCF-43B3-AA09-9EBCB9842492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{B5C7FBEC-5C21-4BB4-BF82-AC400E45706D}"/>
   </bookViews>
@@ -1797,7 +1797,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
+      <selection pane="bottomLeft" activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2248,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1014</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1004</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>992</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>973</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>960</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>922</v>
       </c>

</xml_diff>